<commit_message>
Addaed a new cell
</commit_message>
<xml_diff>
--- a/GIT-FILE-1.xlsx
+++ b/GIT-FILE-1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ravitej/Documents/Git-Training/GIT-Sample/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ravitej/Downloads/Git-Training/GIT-Sample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{71859AF4-8327-0240-9C1C-9A0CE75FC577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4B13DF-65BD-5945-AE1B-C7CA3A44490A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{8840097E-F9E5-C648-A858-4C354906BD0E}"/>
   </bookViews>
@@ -36,9 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Git Smaple</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -410,17 +413,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A518476-2475-064F-968B-85D3B11A789C}">
-  <dimension ref="G16"/>
+  <dimension ref="G16:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="16" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G16" t="s">
         <v>0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>